<commit_message>
div sensete debatter /index.php Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>http://knpbundles.com/KnpLabs/KnpPaginatorBundle</t>
+  </si>
+  <si>
+    <t>temps ecoulé des la creation du debat</t>
+  </si>
+  <si>
+    <t>utilisation de KnpTimeBundle()</t>
+  </si>
+  <si>
+    <t>http://knpbundles.com/KnpLabs/KnpTimeBundle</t>
   </si>
 </sst>
 </file>
@@ -665,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:H11"/>
+  <dimension ref="B4:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B5:H11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,6 +816,21 @@
         <v>29</v>
       </c>
     </row>
+    <row r="12" spans="2:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1"/>
@@ -815,6 +839,7 @@
     <hyperlink ref="H9" r:id="rId4"/>
     <hyperlink ref="H10" r:id="rId5"/>
     <hyperlink ref="H11" r:id="rId6"/>
+    <hyperlink ref="H12" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout style reglé !! Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>http://knpbundles.com/KnpLabs/KnpTimeBundle</t>
+  </si>
+  <si>
+    <t>Editeur de texte (ajout debat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_editeur basique a partir du site http://ckeditor.com/                    _ ajout de Extension Twig personnalisée </t>
+  </si>
+  <si>
+    <t>http://ckeditor.com/</t>
+  </si>
+  <si>
+    <t>utilisation de l extension dans la vue</t>
   </si>
 </sst>
 </file>
@@ -349,9 +361,8 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -385,7 +396,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20 % - Accent1" xfId="6" builtinId="30"/>
@@ -674,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:H12"/>
+  <dimension ref="B4:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,142 +703,159 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:8" s="3" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:8" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="10" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -840,6 +867,7 @@
     <hyperlink ref="H10" r:id="rId5"/>
     <hyperlink ref="H11" r:id="rId6"/>
     <hyperlink ref="H12" r:id="rId7"/>
+    <hyperlink ref="H13" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
validation form ajout style Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -141,6 +141,18 @@
   </si>
   <si>
     <t>avec Request $request je recupere les valeurs des inputs , après validation je persiste</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>validation des champs de Form</t>
+  </si>
+  <si>
+    <t>annotations personnalisés + pattern html5</t>
+  </si>
+  <si>
+    <t>http://www.forma-tice.net/controle-saisie-formulaires/</t>
   </si>
 </sst>
 </file>
@@ -367,7 +379,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,6 +416,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20 % - Accent1" xfId="6" builtinId="30"/>
@@ -692,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:H14"/>
+  <dimension ref="A4:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="B5:H14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,8 +726,9 @@
     <col min="8" max="8" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:8" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -734,7 +751,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -753,7 +771,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -770,7 +789,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -787,7 +807,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
@@ -804,7 +825,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
@@ -819,7 +841,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
@@ -834,7 +857,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
       <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
@@ -849,7 +873,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
         <v>33</v>
       </c>
@@ -866,7 +891,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
       <c r="B14" s="11" t="s">
         <v>37</v>
       </c>
@@ -880,6 +906,24 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="15" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -891,6 +935,7 @@
     <hyperlink ref="H11" r:id="rId6"/>
     <hyperlink ref="H12" r:id="rId7"/>
     <hyperlink ref="H13" r:id="rId8"/>
+    <hyperlink ref="H15" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
repository article fixed and NO fixed position Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>http://www.forma-tice.net/controle-saisie-formulaires/</t>
+  </si>
+  <si>
+    <t>afficher les tag associés au sujet</t>
+  </si>
+  <si>
+    <t>requete join+tableau multi dimension + convert array to sring in twig</t>
+  </si>
+  <si>
+    <t>http://twig.sensiolabs.org/doc/filters/join.html</t>
   </si>
 </sst>
 </file>
@@ -708,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H15"/>
+  <dimension ref="A4:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,6 +934,24 @@
         <v>42</v>
       </c>
     </row>
+    <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="13">
+        <v>42068</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1"/>
@@ -936,6 +963,7 @@
     <hyperlink ref="H12" r:id="rId7"/>
     <hyperlink ref="H13" r:id="rId8"/>
     <hyperlink ref="H15" r:id="rId9"/>
+    <hyperlink ref="H16" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sous meu dynamique selon la page Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>http://twig.sensiolabs.org/doc/filters/join.html</t>
+  </si>
+  <si>
+    <t>sous menu dynamique selon la page courante</t>
+  </si>
+  <si>
+    <t>controlleur imbriqué , etapp.request.get('_route')</t>
+  </si>
+  <si>
+    <t>http://www.developpez.net/forums</t>
+  </si>
+  <si>
+    <t>reponse a ma question dans le forum</t>
   </si>
 </sst>
 </file>
@@ -717,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H16"/>
+  <dimension ref="A4:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,6 +964,26 @@
         <v>45</v>
       </c>
     </row>
+    <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="13">
+        <v>42069</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1"/>
@@ -964,6 +996,7 @@
     <hyperlink ref="H13" r:id="rId8"/>
     <hyperlink ref="H15" r:id="rId9"/>
     <hyperlink ref="H16" r:id="rId10"/>
+    <hyperlink ref="H17" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
formulaire edit reduite !! Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -167,13 +167,28 @@
     <t>sous menu dynamique selon la page courante</t>
   </si>
   <si>
-    <t>controlleur imbriqué , etapp.request.get('_route')</t>
-  </si>
-  <si>
     <t>http://www.developpez.net/forums</t>
   </si>
   <si>
-    <t>reponse a ma question dans le forum</t>
+    <t>trouver la premiere position libre pour un nouveau article</t>
+  </si>
+  <si>
+    <t>Algorithmique pur</t>
+  </si>
+  <si>
+    <t>http://php.net/manual/fr/function.in-array.php</t>
+  </si>
+  <si>
+    <t>controlleur imbriqué , et app.request.get('_route')</t>
+  </si>
+  <si>
+    <t>special Edit : changer les tags de sujet sans afficher tout le form</t>
+  </si>
+  <si>
+    <t>recuperer les anciens valeurs et les renvoyer avec la nouvelle form (reduite )</t>
+  </si>
+  <si>
+    <t>reponse a ma question dans le forum developez.net</t>
   </si>
 </sst>
 </file>
@@ -729,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H17"/>
+  <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +758,7 @@
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -971,18 +986,52 @@
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E17" s="13">
         <v>42069</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>48</v>
-      </c>
+      <c r="E18" s="13">
+        <v>42069</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13">
+        <v>42069</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -997,6 +1046,7 @@
     <hyperlink ref="H15" r:id="rId9"/>
     <hyperlink ref="H16" r:id="rId10"/>
     <hyperlink ref="H17" r:id="rId11"/>
+    <hyperlink ref="H18" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
notification Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>reponse a ma question dans le forum developez.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afficher nombre notif selon le user connecté </t>
+  </si>
+  <si>
+    <t>{%render%}+{%include%}+secureAction</t>
+  </si>
+  <si>
+    <t>http://symfony.com/</t>
+  </si>
+  <si>
+    <t>avec requete count je calcul number notif que jenvoie a une vue , ensuite partout renderController</t>
   </si>
 </sst>
 </file>
@@ -415,7 +427,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -450,12 +462,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20 % - Accent1" xfId="6" builtinId="30"/>
@@ -744,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H19"/>
+  <dimension ref="A4:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +776,7 @@
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -788,7 +800,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -808,7 +820,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -826,7 +838,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -844,7 +856,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="1"/>
       <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
@@ -862,7 +874,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="1"/>
       <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
@@ -878,7 +890,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="1"/>
       <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
@@ -894,7 +906,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="1"/>
       <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
@@ -910,7 +922,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="1"/>
       <c r="B13" s="11" t="s">
         <v>33</v>
       </c>
@@ -928,110 +940,130 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="1"/>
       <c r="B14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="11" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="13">
         <v>42067</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="15" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="1"/>
       <c r="B16" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="1"/>
       <c r="D16" s="11" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="13">
         <v>42068</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="15" t="s">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="1"/>
       <c r="B17" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E17" s="13">
         <v>42069</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12" t="s">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="1"/>
       <c r="B18" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="11" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="13">
         <v>42069</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="15" t="s">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="1"/>
       <c r="B19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="13">
         <v>42069</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="12"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="13">
+        <v>42073</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1047,6 +1079,7 @@
     <hyperlink ref="H16" r:id="rId10"/>
     <hyperlink ref="H17" r:id="rId11"/>
     <hyperlink ref="H18" r:id="rId12"/>
+    <hyperlink ref="H20" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout de Services partout !! Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>avec requete count je calcul number notif que jenvoie a une vue , ensuite partout renderController</t>
+  </si>
+  <si>
+    <t>gestion flexible des entités</t>
+  </si>
+  <si>
+    <t>Utilisation des Services</t>
   </si>
 </sst>
 </file>
@@ -756,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H20"/>
+  <dimension ref="A4:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="A5:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,6 +1071,22 @@
         <v>57</v>
       </c>
     </row>
+    <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="13">
+        <v>42074</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1"/>

</xml_diff>

<commit_message>
notification reglé definitivement :D Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Utilisation des Services</t>
+  </si>
+  <si>
+    <t>gestion de Notification si coché lors de l ajout de new Topic</t>
   </si>
 </sst>
 </file>
@@ -762,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H21"/>
+  <dimension ref="A4:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="A5:H21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B22" sqref="A5:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,6 +1090,22 @@
       </c>
       <c r="H21" s="1"/>
     </row>
+    <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="13">
+        <v>42074</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1"/>

</xml_diff>

<commit_message>
probleme des objets supprimés avec image Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -210,13 +210,19 @@
   </si>
   <si>
     <t>gestion de Notification si coché lors de l ajout de new Topic</t>
+  </si>
+  <si>
+    <t>affecter l'AR a sa position choisi et si pos=1 , on l'affecte a la premiere libre</t>
+  </si>
+  <si>
+    <t>https://php.net/manual/fr/index.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,27 +287,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -312,24 +297,69 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -436,45 +466,48 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -765,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H22"/>
+  <dimension ref="A4:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B22" sqref="A5:H22"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,327 +817,345 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="11" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="10" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="10" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="10" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="14">
         <v>42067</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="10" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="14">
         <v>42068</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="10" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="11" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="14">
         <v>42069</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="11" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="14">
         <v>42069</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="10" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="13">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14">
         <v>42069</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
+      <c r="F19" s="11"/>
+      <c r="G19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="14">
         <v>42073</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="13">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="14">
         <v>42074</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="11" t="s">
+      <c r="F21" s="11"/>
+      <c r="G21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="13">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="14">
         <v>42074</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="11" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="14">
+        <v>42079</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1121,6 +1172,7 @@
     <hyperlink ref="H17" r:id="rId11"/>
     <hyperlink ref="H18" r:id="rId12"/>
     <hyperlink ref="H20" r:id="rId13"/>
+    <hyperlink ref="H23" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
gestion des Threads /administration Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -216,13 +216,31 @@
   </si>
   <si>
     <t>https://php.net/manual/fr/index.php</t>
+  </si>
+  <si>
+    <t>afficher le champs de commentaire si je clique "add comment"</t>
+  </si>
+  <si>
+    <t>Jquery - ui</t>
+  </si>
+  <si>
+    <t>http://jqueryui.com/toggle/</t>
+  </si>
+  <si>
+    <t>gestion des treads</t>
+  </si>
+  <si>
+    <t>http://php.net/manual/fr/function.array-values.php</t>
+  </si>
+  <si>
+    <t>recuperer les valeurs de form dans un tableau , les comparer aux valeurs de tableau Sujet-&gt;getThread sinon update</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +315,66 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -309,48 +385,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -466,49 +501,55 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -798,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H23"/>
+  <dimension ref="A4:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="C25" sqref="A5:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,343 +859,379 @@
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="13" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13" t="s">
+    <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>42067</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>42068</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>42069</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="13" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>42069</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13">
         <v>42069</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="13" t="s">
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <v>42073</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="14">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13">
         <v>42074</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="13" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="13" t="s">
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13">
         <v>42074</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="13" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="13" t="s">
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="13">
         <v>42079</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="2" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="13">
+        <v>42081</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15">
+        <v>42081</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1173,6 +1250,8 @@
     <hyperlink ref="H18" r:id="rId12"/>
     <hyperlink ref="H20" r:id="rId13"/>
     <hyperlink ref="H23" r:id="rId14"/>
+    <hyperlink ref="H24" r:id="rId15"/>
+    <hyperlink ref="H25" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adddstyle validation des inputs couleurs Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -227,13 +227,19 @@
     <t>http://jqueryui.com/toggle/</t>
   </si>
   <si>
-    <t>gestion des treads</t>
-  </si>
-  <si>
     <t>http://php.net/manual/fr/function.array-values.php</t>
   </si>
   <si>
     <t>recuperer les valeurs de form dans un tableau , les comparer aux valeurs de tableau Sujet-&gt;getThread sinon update</t>
+  </si>
+  <si>
+    <t>gestion des threads</t>
+  </si>
+  <si>
+    <t>validator pattern pour code couleur (add style)</t>
+  </si>
+  <si>
+    <t>http://www.infraworld.fr/2014/10/07/validation-de-formulaire-sans-javascript-avec-html5/</t>
   </si>
 </sst>
 </file>
@@ -380,17 +386,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <u/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -543,13 +547,13 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="16" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -839,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H25"/>
+  <dimension ref="A4:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="C25" sqref="A5:H25"/>
+      <selection activeCell="B26" sqref="A5:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,21 +1221,37 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="13">
+        <v>42081</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15">
+    </row>
+    <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15">
         <v>42081</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>68</v>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="16" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1252,6 +1272,7 @@
     <hyperlink ref="H23" r:id="rId14"/>
     <hyperlink ref="H24" r:id="rId15"/>
     <hyperlink ref="H25" r:id="rId16"/>
+    <hyperlink ref="H26" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cacher les input addcomment si je clique "annuler" Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>http://www.infraworld.fr/2014/10/07/validation-de-formulaire-sans-javascript-avec-html5/</t>
+  </si>
+  <si>
+    <t>show -hide thread comment on click</t>
+  </si>
+  <si>
+    <t>http://api.jquery.com/</t>
   </si>
 </sst>
 </file>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H26"/>
+  <dimension ref="A4:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="B26" sqref="A5:H26"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="B27" sqref="A5:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,6 +1260,22 @@
         <v>71</v>
       </c>
     </row>
+    <row r="27" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15">
+        <v>42087</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1"/>
@@ -1273,6 +1295,7 @@
     <hyperlink ref="H24" r:id="rId15"/>
     <hyperlink ref="H25" r:id="rId16"/>
     <hyperlink ref="H26" r:id="rId17"/>
+    <hyperlink ref="H27" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update tag input texte Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -246,13 +246,19 @@
   </si>
   <si>
     <t>http://api.jquery.com/</t>
+  </si>
+  <si>
+    <t>validation password strenght</t>
+  </si>
+  <si>
+    <t>http://www.w3schools.com/tags/att_input_pattern.asp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,64 +332,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <u/>
       <sz val="14"/>
       <color theme="10"/>
@@ -396,15 +351,42 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+    </font>
+    <font>
       <sz val="14"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -519,46 +501,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -849,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H27"/>
+  <dimension ref="A4:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="B27" sqref="A5:H27"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="B28" sqref="A5:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,411 +851,427 @@
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="12" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="3">
         <v>42067</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="3">
         <v>42068</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="3">
         <v>42069</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="3">
         <v>42069</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11" t="s">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="13">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3">
         <v>42069</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="10"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12" t="s">
+      <c r="A20" s="2"/>
+      <c r="B20" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="3">
         <v>42073</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="12" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3">
         <v>42074</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="12" t="s">
+      <c r="F21" s="2"/>
+      <c r="G21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="10"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3">
         <v>42074</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="12" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="10"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="3">
         <v>42079</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="12" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="3">
         <v>42081</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11" t="s">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="12" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="13">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3">
         <v>42081</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="12" t="s">
+      <c r="F25" s="2"/>
+      <c r="G25" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3">
         <v>42081</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="16" t="s">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="12" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3">
         <v>42087</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="16" t="s">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="4" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15">
+        <v>42089</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="16" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1296,6 +1294,7 @@
     <hyperlink ref="H25" r:id="rId16"/>
     <hyperlink ref="H26" r:id="rId17"/>
     <hyperlink ref="H27" r:id="rId18"/>
+    <hyperlink ref="H28" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
shift left right not yet Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -252,13 +252,25 @@
   </si>
   <si>
     <t>http://www.w3schools.com/tags/att_input_pattern.asp</t>
+  </si>
+  <si>
+    <t>control d'affectation de AR (backend)</t>
+  </si>
+  <si>
+    <t>recuperer l'array request et le comparer a lui-même avec  array_unique</t>
+  </si>
+  <si>
+    <t>http://php.net/manual/fr/function.array-unique.php</t>
+  </si>
+  <si>
+    <t>algorithmique pur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,13 +344,72 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <u/>
       <sz val="14"/>
       <color theme="10"/>
@@ -347,46 +418,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -498,49 +536,49 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -831,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H28"/>
+  <dimension ref="A4:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="B28" sqref="A5:H28"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,416 +889,416 @@
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="13" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="13">
         <v>42067</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="4" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="13">
         <v>42068</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="4" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="13">
         <v>42069</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="13" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="13">
         <v>42069</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="4" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="10"/>
+      <c r="B19" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13">
         <v>42069</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="13">
         <v>42073</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13">
         <v>42074</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="13" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13">
         <v>42074</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="13" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="13">
         <v>42079</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="4" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="13">
         <v>42081</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="4" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="13">
         <v>42081</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="13" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="13">
         <v>42081</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="4" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="13" t="s">
+      <c r="A27" s="10"/>
+      <c r="B27" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13">
         <v>42087</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="4" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>74</v>
       </c>
       <c r="C28" s="14"/>
@@ -1272,6 +1310,26 @@
       <c r="G28" s="14"/>
       <c r="H28" s="16" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="15">
+        <v>42093</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1295,6 +1353,7 @@
     <hyperlink ref="H26" r:id="rId17"/>
     <hyperlink ref="H27" r:id="rId18"/>
     <hyperlink ref="H28" r:id="rId19"/>
+    <hyperlink ref="H29" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
shift to left ARs if add shift to right ARs if delete Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>algorithmique pur</t>
+  </si>
+  <si>
+    <t>shift to right if add shift to left if delete</t>
   </si>
 </sst>
 </file>
@@ -869,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H29"/>
+  <dimension ref="A4:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="C30" sqref="A5:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,6 +1334,22 @@
       <c r="H29" s="16" t="s">
         <v>78</v>
       </c>
+    </row>
+    <row r="30" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="15">
+        <v>42094</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
correction input ajout comment Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -267,6 +267,15 @@
   </si>
   <si>
     <t>shift to right if add shift to left if delete</t>
+  </si>
+  <si>
+    <t>http://www.webcodegeeks.com/javascript/jquery/jquery-tooltip-example/</t>
+  </si>
+  <si>
+    <t>affichage de tooltip UserDetails dans partie forum</t>
+  </si>
+  <si>
+    <t>JS+CSS</t>
   </si>
 </sst>
 </file>
@@ -872,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H30"/>
+  <dimension ref="A4:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="C30" sqref="A5:H30"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="C31" sqref="A5:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,6 +1359,24 @@
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="15">
+        <v>42096</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="16" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1373,6 +1400,7 @@
     <hyperlink ref="H27" r:id="rId18"/>
     <hyperlink ref="H28" r:id="rId19"/>
     <hyperlink ref="H29" r:id="rId20"/>
+    <hyperlink ref="H31" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tous les tooltip sont reglés :D Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>JS+CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage de tooltip si user click add new comment hors non connecté  </t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -591,6 +594,15 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -881,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H31"/>
+  <dimension ref="A4:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="C31" sqref="A5:H31"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="B32" sqref="A5:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,6 +1389,22 @@
       <c r="H31" s="16" t="s">
         <v>81</v>
       </c>
+    </row>
+    <row r="32" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="19">
+        <v>42100</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
design tooltip sujetrecent Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t xml:space="preserve">affichage de tooltip si user click add new comment hors non connecté  </t>
+  </si>
+  <si>
+    <t>http://jquery-plugins.net/tokenfield-jquery-tag-token-plugin-for-bootstrap</t>
+  </si>
+  <si>
+    <t>autocomplete des tags pendant l ajout de nouveau sujet</t>
+  </si>
+  <si>
+    <t>JS+JQ+CSS+bootstrap 3</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -596,13 +605,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H32"/>
+  <dimension ref="A4:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="B32" sqref="A5:H32"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,20 +1394,38 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18" t="s">
+      <c r="C32" s="14"/>
+      <c r="D32" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="15">
         <v>42100</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14"/>
+      <c r="B33" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="15">
+        <v>42100</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="16" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1429,6 +1450,7 @@
     <hyperlink ref="H28" r:id="rId19"/>
     <hyperlink ref="H29" r:id="rId20"/>
     <hyperlink ref="H31" r:id="rId21"/>
+    <hyperlink ref="H33" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
deux ckeditor Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -288,6 +288,15 @@
   </si>
   <si>
     <t>JS+JQ+CSS+bootstrap 3</t>
+  </si>
+  <si>
+    <t>affichage du contenu de Ckeditor (html interpreté)</t>
+  </si>
+  <si>
+    <t>fitre |raw</t>
+  </si>
+  <si>
+    <t>http://twig.sensiolabs.org/doc/filters/raw.html</t>
   </si>
 </sst>
 </file>
@@ -896,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H33"/>
+  <dimension ref="A4:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="B34" sqref="A5:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,6 +1434,24 @@
       <c r="G33" s="14"/>
       <c r="H33" s="16" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
+      <c r="B34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="15">
+        <v>42107</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1451,6 +1478,7 @@
     <hyperlink ref="H29" r:id="rId20"/>
     <hyperlink ref="H31" r:id="rId21"/>
     <hyperlink ref="H33" r:id="rId22"/>
+    <hyperlink ref="H34" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
afficher image selon User src Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -297,13 +297,25 @@
   </si>
   <si>
     <t>http://twig.sensiolabs.org/doc/filters/raw.html</t>
+  </si>
+  <si>
+    <t>change-password controller ne connait pas "em"</t>
+  </si>
+  <si>
+    <t>public function getDoctrine()
+{
+    return $this-&gt;container-&gt;get('doctrine');
+}</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/22841440/symfony2-call-to-undefined-method-getdoctrine-when-overriding-fosuserbundle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,78 +398,61 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -564,46 +559,10 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -611,10 +570,34 @@
     <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -905,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H34"/>
+  <dimension ref="A4:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="B34" sqref="A5:H34"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="B35" sqref="A5:H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,533 +908,551 @@
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="12" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="12" t="s">
+    <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="3">
         <v>42067</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="12" t="s">
+    <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="3">
         <v>42068</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="3">
         <v>42069</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12" t="s">
+    <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="3">
         <v>42069</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11" t="s">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="13">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3">
         <v>42069</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12" t="s">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="3">
         <v>42073</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="12" t="s">
+    <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3">
         <v>42074</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="12" t="s">
+      <c r="F21" s="2"/>
+      <c r="G21" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12" t="s">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3">
         <v>42074</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="12" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12" t="s">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="3">
         <v>42079</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="12" t="s">
+    <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="3">
         <v>42081</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11" t="s">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="12" t="s">
+    <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="13">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3">
         <v>42081</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="12" t="s">
+      <c r="F25" s="2"/>
+      <c r="G25" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="12" t="s">
+    <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="13">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3">
         <v>42081</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11" t="s">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="12" t="s">
+    <row r="27" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3">
         <v>42087</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11" t="s">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="12" t="s">
+    <row r="28" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3">
         <v>42089</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="16" t="s">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="12" t="s">
+    <row r="29" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="3">
         <v>42093</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14" t="s">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="12" t="s">
+    <row r="30" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14" t="s">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="3">
         <v>42094</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="12" t="s">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14" t="s">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="3">
         <v>42096</v>
       </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="16" t="s">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="12" t="s">
+    <row r="32" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="17" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="3">
         <v>42100</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="12" t="s">
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="17" t="s">
+      <c r="C33" s="2"/>
+      <c r="D33" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="3">
         <v>42100</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="16" t="s">
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="12" t="s">
+    <row r="34" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="17" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="3">
         <v>42107</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="16" t="s">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="4" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="3">
+        <v>42107</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1479,6 +1480,7 @@
     <hyperlink ref="H31" r:id="rId21"/>
     <hyperlink ref="H33" r:id="rId22"/>
     <hyperlink ref="H34" r:id="rId23"/>
+    <hyperlink ref="H35" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
frontpage Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>http://stackoverflow.com/questions/22841440/symfony2-call-to-undefined-method-getdoctrine-when-overriding-fosuserbundle</t>
+  </si>
+  <si>
+    <t>afficher div topic les plus commentés</t>
+  </si>
+  <si>
+    <t>http://php.net/manual/fr/function.rsort.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">algorithmique : for , array_push,rsort </t>
   </si>
 </sst>
 </file>
@@ -888,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H35"/>
+  <dimension ref="A4:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="B35" sqref="A5:H35"/>
+    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="C36" sqref="A5:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,6 +1462,24 @@
       <c r="G35" s="2"/>
       <c r="H35" s="4" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="3">
+        <v>42109</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1481,6 +1508,7 @@
     <hyperlink ref="H33" r:id="rId22"/>
     <hyperlink ref="H34" r:id="rId23"/>
     <hyperlink ref="H35" r:id="rId24"/>
+    <hyperlink ref="H36" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
div last news in frontpage :) Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t xml:space="preserve">algorithmique : for , array_push,rsort </t>
+  </si>
+  <si>
+    <t>construire nouveau sujet a partir de article</t>
+  </si>
+  <si>
+    <t>routing , default text field value</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/13916001/set-default-value-of-symfony-2-form-field-in-twig</t>
   </si>
 </sst>
 </file>
@@ -897,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H36"/>
+  <dimension ref="A4:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="C36" sqref="A5:H36"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="C37" sqref="A5:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,6 +1489,24 @@
       <c r="G36" s="2"/>
       <c r="H36" s="4" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="3">
+        <v>42110</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1509,6 +1536,7 @@
     <hyperlink ref="H34" r:id="rId23"/>
     <hyperlink ref="H35" r:id="rId24"/>
     <hyperlink ref="H36" r:id="rId25"/>
+    <hyperlink ref="H37" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
translation droite AR Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>http://stackoverflow.com/questions/13916001/set-default-value-of-symfony-2-form-field-in-twig</t>
+  </si>
+  <si>
+    <t>Episode 25 -DevAndClick Chaine Youtube</t>
+  </si>
+  <si>
+    <t>gerer image upload ( add , update )</t>
   </si>
 </sst>
 </file>
@@ -577,7 +583,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -616,6 +622,12 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -906,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H37"/>
+  <dimension ref="A4:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
-      <selection activeCell="C37" sqref="A5:H37"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="B38" sqref="A5:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,6 +1519,22 @@
       <c r="G37" s="2"/>
       <c r="H37" s="4" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="15">
+        <v>42121</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction des gestion des positions AR Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="107">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>affichage du contenu de Ckeditor (html interpreté)</t>
-  </si>
-  <si>
-    <t>fitre |raw</t>
   </si>
   <si>
     <t>http://twig.sensiolabs.org/doc/filters/raw.html</t>
@@ -333,6 +330,24 @@
   </si>
   <si>
     <t>gerer image upload ( add , update )</t>
+  </si>
+  <si>
+    <t>afficher liste debat les plus commentés par nomre de comments</t>
+  </si>
+  <si>
+    <t>20_avr</t>
+  </si>
+  <si>
+    <t>Algorithmique , requete QueryBuilder</t>
+  </si>
+  <si>
+    <t>afficher liste debat ne sont pas crés a partir des 15 AR</t>
+  </si>
+  <si>
+    <t>filtre |raw</t>
+  </si>
+  <si>
+    <t>notification pour user createur de sujet [X] si on le commente avec couleur vu et non vu</t>
   </si>
 </sst>
 </file>
@@ -624,11 +639,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -918,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H38"/>
+  <dimension ref="A4:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="B38" sqref="A5:H38"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="B41" sqref="A5:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1471,7 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="5" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="E34" s="3">
         <v>42107</v>
@@ -1464,17 +1479,17 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E35" s="3">
         <v>42107</v>
@@ -1482,17 +1497,17 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E36" s="3">
         <v>42109</v>
@@ -1500,17 +1515,17 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E37" s="3">
         <v>42110</v>
@@ -1518,24 +1533,72 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3">
+        <v>42121</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="5" t="s">
+    <row r="39" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="15">
-        <v>42121</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14" t="s">
-        <v>100</v>
-      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="3">
+        <v>42113</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="15">
+        <v>42119</v>
+      </c>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Style Bannieres Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -348,6 +348,18 @@
   </si>
   <si>
     <t>notification pour user createur de sujet [X] si on le commente avec couleur vu et non vu</t>
+  </si>
+  <si>
+    <t>ajout de lextension Slug pour Debat</t>
+  </si>
+  <si>
+    <t>nouveau attribut Slug generé a partir de Sujet et qui est a l'URL</t>
+  </si>
+  <si>
+    <t>http://tutorial.symblog.co.uk/docs/customising-the-view-more-with-twig.html#slugifying-the-url</t>
+  </si>
+  <si>
+    <t>Bundle :DoctrineExtensionsBundle</t>
   </si>
 </sst>
 </file>
@@ -598,7 +610,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -639,11 +651,14 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -933,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H41"/>
+  <dimension ref="A4:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="B41" sqref="A5:H41"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,20 +1600,40 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C41" s="14"/>
+      <c r="C41" s="2"/>
       <c r="D41" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="3">
         <v>42119</v>
       </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="15">
+        <v>42123</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1628,6 +1663,7 @@
     <hyperlink ref="H35" r:id="rId24"/>
     <hyperlink ref="H36" r:id="rId25"/>
     <hyperlink ref="H37" r:id="rId26"/>
+    <hyperlink ref="H42" r:id="rId27" location="slugifying-the-url"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add menu selon des lien ( routing ) Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>Bundle :DoctrineExtensionsBundle</t>
+  </si>
+  <si>
+    <t>ajout de rubrique menu a partir des routing existants dans le projet</t>
+  </si>
+  <si>
+    <t>parcourir toutes les routes et les injecter dans formBuilder</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -649,15 +655,6 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -948,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H42"/>
+  <dimension ref="A4:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="C43" sqref="A5:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,24 +1613,40 @@
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="14"/>
+      <c r="C42" s="2"/>
       <c r="D42" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="3">
         <v>42123</v>
       </c>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14" t="s">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="4" t="s">
         <v>109</v>
       </c>
+    </row>
+    <row r="43" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="3">
+        <v>42126</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ajax Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -366,6 +366,15 @@
   </si>
   <si>
     <t>parcourir toutes les routes et les injecter dans formBuilder</t>
+  </si>
+  <si>
+    <t>ajout avec ajax</t>
+  </si>
+  <si>
+    <t>08_mai</t>
+  </si>
+  <si>
+    <t>http://www.xul.fr/scripts/</t>
   </si>
 </sst>
 </file>
@@ -616,7 +625,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -655,6 +664,12 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -945,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H43"/>
+  <dimension ref="A4:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
-      <selection activeCell="C43" sqref="A5:H43"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="B44" sqref="A5:H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,6 +1662,22 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="15" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1677,6 +1708,7 @@
     <hyperlink ref="H36" r:id="rId25"/>
     <hyperlink ref="H37" r:id="rId26"/>
     <hyperlink ref="H42" r:id="rId27" location="slugifying-the-url"/>
+    <hyperlink ref="H44" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout de Bundle FOSJSrouting necessaire pour ajax Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -371,10 +371,19 @@
     <t>ajout avec ajax</t>
   </si>
   <si>
-    <t>08_mai</t>
-  </si>
-  <si>
-    <t>http://www.xul.fr/scripts/</t>
+    <t>http://www.xul.fr/scripts/  et  http://y-btk.blogspot.com/2014/12/les-controleurs-avec-symfony2.html   et     http://openclassrooms.com/forum/sujet/symfony-formulaire-dynamique-cadeau</t>
+  </si>
+  <si>
+    <t>utiliser probablement le Bundle FOSJSrouting</t>
+  </si>
+  <si>
+    <t>chargement des pages lent</t>
+  </si>
+  <si>
+    <t>http://openclassrooms.com/courses/accelerer-la-generation-de-vos-pages-php-avec-l-extension-apc</t>
+  </si>
+  <si>
+    <t>install  et config de APC dans wamp</t>
   </si>
 </sst>
 </file>
@@ -625,7 +634,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -664,12 +673,6 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -960,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H44"/>
+  <dimension ref="A4:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="B44" sqref="A5:H44"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="B45" sqref="A5:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,19 +1667,39 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14" t="s">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="3">
+        <v>42132</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="15" t="s">
-        <v>115</v>
+    </row>
+    <row r="45" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="3">
+        <v>42124</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +1731,8 @@
     <hyperlink ref="H36" r:id="rId25"/>
     <hyperlink ref="H37" r:id="rId26"/>
     <hyperlink ref="H42" r:id="rId27" location="slugifying-the-url"/>
-    <hyperlink ref="H44" r:id="rId28"/>
+    <hyperlink ref="H44" r:id="rId28" display="http://www.xul.fr/scripts/"/>
+    <hyperlink ref="H45" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correction tag pour nouveau debat Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="122">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -384,6 +384,15 @@
   </si>
   <si>
     <t>install  et config de APC dans wamp</t>
+  </si>
+  <si>
+    <t>hide div  (tooltip) if click outside</t>
+  </si>
+  <si>
+    <t>JQUery code</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/1403615/use-jquery-to-hide-a-div-when-the-user-clicks-outside-of-it</t>
   </si>
 </sst>
 </file>
@@ -639,41 +648,41 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -963,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H45"/>
+  <dimension ref="A4:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
-      <selection activeCell="B45" sqref="A5:H45"/>
+      <selection activeCell="B46" sqref="A5:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,723 +992,741 @@
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="5" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="13">
         <v>42067</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="4" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="13">
         <v>42068</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="4" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="13">
         <v>42069</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="13">
         <v>42069</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="4" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="10"/>
+      <c r="B19" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13">
         <v>42069</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="13">
         <v>42073</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13">
         <v>42074</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="5" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13">
         <v>42074</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="5" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="13">
         <v>42079</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="4" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="13">
         <v>42081</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="4" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="13">
         <v>42081</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="5" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="13">
         <v>42081</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="4" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="10"/>
+      <c r="B27" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13">
         <v>42087</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="4" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="10"/>
+      <c r="B28" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="13">
         <v>42089</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="4" t="s">
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="13">
         <v>42093</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2" t="s">
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="13">
         <v>42094</v>
       </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="10"/>
+      <c r="B31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="13">
         <v>42096</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="4" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="11" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="10"/>
+      <c r="B32" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="5" t="s">
+      <c r="C32" s="10"/>
+      <c r="D32" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="13">
         <v>42100</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="10"/>
+      <c r="D33" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="13">
         <v>42100</v>
       </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="4" t="s">
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="10"/>
+      <c r="B34" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="5" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="13">
         <v>42107</v>
       </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="4" t="s">
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="10"/>
+      <c r="B35" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
+      <c r="C35" s="10"/>
+      <c r="D35" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="13">
         <v>42107</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="4" t="s">
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="11" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="10"/>
+      <c r="B36" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="5" t="s">
+      <c r="C36" s="10"/>
+      <c r="D36" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="13">
         <v>42109</v>
       </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="4" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="5" t="s">
+      <c r="C37" s="10"/>
+      <c r="D37" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="13">
         <v>42110</v>
       </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="4" t="s">
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="10"/>
+      <c r="B38" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="13">
         <v>42121</v>
       </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2" t="s">
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="10"/>
+      <c r="B39" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="5" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="5" t="s">
+      <c r="A40" s="10"/>
+      <c r="B40" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="5" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="13">
         <v>42113</v>
       </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="10"/>
+      <c r="B41" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="5" t="s">
+      <c r="C41" s="10"/>
+      <c r="D41" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="13">
         <v>42119</v>
       </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="10"/>
+      <c r="B42" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="5" t="s">
+      <c r="C42" s="10"/>
+      <c r="D42" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="13">
         <v>42123</v>
       </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2" t="s">
+      <c r="F42" s="10"/>
+      <c r="G42" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="5" t="s">
+      <c r="A43" s="10"/>
+      <c r="B43" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="5" t="s">
+      <c r="C43" s="10"/>
+      <c r="D43" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="13">
         <v>42126</v>
       </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="10"/>
+      <c r="B44" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
+      <c r="C44" s="10"/>
+      <c r="D44" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="13">
         <v>42132</v>
       </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="4" t="s">
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="10"/>
+      <c r="B45" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="5" t="s">
+      <c r="C45" s="10"/>
+      <c r="D45" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="13">
         <v>42124</v>
       </c>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="4" t="s">
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="11" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" s="13">
+        <v>42139</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="11" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1733,6 +1760,7 @@
     <hyperlink ref="H42" r:id="rId27" location="slugifying-the-url"/>
     <hyperlink ref="H44" r:id="rId28" display="http://www.xul.fr/scripts/"/>
     <hyperlink ref="H45" r:id="rId29"/>
+    <hyperlink ref="H46" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
effet hover img Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -393,13 +393,19 @@
   </si>
   <si>
     <t>http://stackoverflow.com/questions/1403615/use-jquery-to-hide-a-div-when-the-user-clicks-outside-of-it</t>
+  </si>
+  <si>
+    <t>design:rotate img on hover</t>
+  </si>
+  <si>
+    <t>http://blog.vivekv.com/rotate-image-360deg-when-mouse-hover-using-css-3.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,66 +479,42 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -648,41 +630,41 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -972,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H46"/>
+  <dimension ref="A4:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
-      <selection activeCell="B46" sqref="A5:H46"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="C47" sqref="A5:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,6 +1709,22 @@
       <c r="G46" s="10"/>
       <c r="H46" s="11" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="13">
+        <v>42140</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="11" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1761,6 +1759,7 @@
     <hyperlink ref="H44" r:id="rId28" display="http://www.xul.fr/scripts/"/>
     <hyperlink ref="H45" r:id="rId29"/>
     <hyperlink ref="H46" r:id="rId30"/>
+    <hyperlink ref="H47" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit comment Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="126">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -399,13 +399,19 @@
   </si>
   <si>
     <t>http://blog.vivekv.com/rotate-image-360deg-when-mouse-hover-using-css-3.html</t>
+  </si>
+  <si>
+    <t>ckeditor vider apres chaque submit</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/5442646/how-to-clear-ckeditor-form-after-submiting-with-ajax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,46 +485,70 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -625,47 +655,50 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20 % - Accent1" xfId="6" builtinId="30"/>
@@ -954,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H47"/>
+  <dimension ref="A4:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
-      <selection activeCell="C47" sqref="A5:H47"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="B48" sqref="A5:H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,6 +1758,22 @@
       <c r="G47" s="10"/>
       <c r="H47" s="11" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="15">
+        <v>42149</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="16" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1760,6 +1809,7 @@
     <hyperlink ref="H45" r:id="rId29"/>
     <hyperlink ref="H46" r:id="rId30"/>
     <hyperlink ref="H47" r:id="rId31"/>
+    <hyperlink ref="H48" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
horos flux et jquery Signed-off-by: MehezLabidi <mehrez.labidi@esprit.tn>
</commit_message>
<xml_diff>
--- a/Remarque - Problematique.xlsx
+++ b/Remarque - Problematique.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="128">
   <si>
     <t xml:space="preserve">       solution provisoire</t>
   </si>
@@ -405,6 +405,12 @@
   </si>
   <si>
     <t>http://stackoverflow.com/questions/5442646/how-to-clear-ckeditor-form-after-submiting-with-ajax</t>
+  </si>
+  <si>
+    <t>anim horo</t>
+  </si>
+  <si>
+    <t>http://www.creativejuiz.fr/blog/tutoriels/infinite-slideshow-quelques-lignes-jquery</t>
   </si>
 </sst>
 </file>
@@ -655,50 +661,59 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20 % - Accent1" xfId="6" builtinId="30"/>
@@ -987,793 +1002,810 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H48"/>
+  <dimension ref="A4:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="B48" sqref="A5:H48"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="12" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="14">
         <v>42067</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="14">
         <v>42068</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="14">
         <v>42069</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="14">
         <v>42069</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="13">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14">
         <v>42069</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="11"/>
+      <c r="G19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="10"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="14">
         <v>42073</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="12" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="14">
         <v>42074</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="12" t="s">
+      <c r="F21" s="11"/>
+      <c r="G21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="10"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="14">
         <v>42074</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="12" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="10"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="14">
         <v>42079</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11" t="s">
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="12" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="14">
         <v>42081</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11" t="s">
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="12" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="13">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="14">
         <v>42081</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="12" t="s">
+      <c r="F25" s="11"/>
+      <c r="G25" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="13">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="14">
         <v>42081</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11" t="s">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="12" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="14">
         <v>42087</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11" t="s">
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="12" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="13">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="14">
         <v>42089</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11" t="s">
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="12" t="s">
+      <c r="A29" s="11"/>
+      <c r="B29" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="14">
         <v>42093</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="12" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10" t="s">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="14">
         <v>42094</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="12" t="s">
+      <c r="A31" s="11"/>
+      <c r="B31" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10" t="s">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="14">
         <v>42096</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11" t="s">
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="14">
         <v>42100</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="12" t="s">
+      <c r="C33" s="11"/>
+      <c r="D33" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="14">
         <v>42100</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="11" t="s">
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="11"/>
+      <c r="B34" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="12" t="s">
+      <c r="C34" s="11"/>
+      <c r="D34" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="14">
         <v>42107</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="11" t="s">
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10" t="s">
+      <c r="C35" s="11"/>
+      <c r="D35" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="14">
         <v>42107</v>
       </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="11" t="s">
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="12" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="12" t="s">
+      <c r="C36" s="11"/>
+      <c r="D36" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="14">
         <v>42109</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="11" t="s">
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="12" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="12" t="s">
+      <c r="C37" s="11"/>
+      <c r="D37" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="14">
         <v>42110</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="11" t="s">
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="13">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="14">
         <v>42121</v>
       </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10" t="s">
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="12" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="12" t="s">
+      <c r="C39" s="11"/>
+      <c r="D39" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
     </row>
     <row r="40" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="12" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="11"/>
+      <c r="D40" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="14">
         <v>42113</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
     </row>
     <row r="41" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="12" t="s">
+      <c r="C41" s="11"/>
+      <c r="D41" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="14">
         <v>42119</v>
       </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
     </row>
     <row r="42" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="12" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="12" t="s">
+      <c r="C42" s="11"/>
+      <c r="D42" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="14">
         <v>42123</v>
       </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10" t="s">
+      <c r="F42" s="11"/>
+      <c r="G42" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="H42" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="12" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="12" t="s">
+      <c r="C43" s="11"/>
+      <c r="D43" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="14">
         <v>42126</v>
       </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
     </row>
     <row r="44" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="12" t="s">
+      <c r="A44" s="11"/>
+      <c r="B44" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10" t="s">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="14">
         <v>42132</v>
       </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="11" t="s">
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="12" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="12" t="s">
+      <c r="A45" s="11"/>
+      <c r="B45" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="12" t="s">
+      <c r="C45" s="11"/>
+      <c r="D45" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="14">
         <v>42124</v>
       </c>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="11" t="s">
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="11"/>
+      <c r="B46" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="12" t="s">
+      <c r="C46" s="11"/>
+      <c r="D46" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="14">
         <v>42139</v>
       </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="11" t="s">
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="12" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="12" t="s">
+      <c r="A47" s="11"/>
+      <c r="B47" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="13">
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="14">
         <v>42140</v>
       </c>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="11" t="s">
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="12" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="12" t="s">
+      <c r="A48" s="11"/>
+      <c r="B48" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="15">
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="14">
         <v>42149</v>
       </c>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="16" t="s">
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="12" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
+      <c r="B49" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="16">
+        <v>42154</v>
+      </c>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="17" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1810,6 +1842,7 @@
     <hyperlink ref="H46" r:id="rId30"/>
     <hyperlink ref="H47" r:id="rId31"/>
     <hyperlink ref="H48" r:id="rId32"/>
+    <hyperlink ref="H49" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>